<commit_message>
Updated bearing capacity calculation
</commit_message>
<xml_diff>
--- a/cpt_data_p_y_curve.xlsx
+++ b/cpt_data_p_y_curve.xlsx
@@ -571,70 +571,70 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="E2" t="n">
-        <v>30.55698153572829</v>
+        <v>4.30141506619142</v>
       </c>
       <c r="F2" t="n">
-        <v>1.951232399646889</v>
+        <v>17.5</v>
       </c>
       <c r="G2" t="n">
-        <v>51.89144567440538</v>
+        <v>17.20566026476568</v>
       </c>
       <c r="H2" t="n">
-        <v>3.807307877431757</v>
+        <v>38.5</v>
       </c>
       <c r="I2" t="n">
-        <v>70.72820374016646</v>
+        <v>25.80849039714852</v>
       </c>
       <c r="J2" t="n">
-        <v>7.428942485875671</v>
+        <v>73.50000000000001</v>
       </c>
       <c r="K2" t="n">
-        <v>76.36587357632942</v>
+        <v>34.41132052953136</v>
       </c>
       <c r="L2" t="n">
-        <v>14.49559327355391</v>
+        <v>119</v>
       </c>
       <c r="M2" t="n">
-        <v>76.6545992103463</v>
+        <v>43.0141506619142</v>
       </c>
       <c r="N2" t="n">
-        <v>28.28427124746191</v>
+        <v>182</v>
       </c>
       <c r="O2" t="n">
-        <v>76.6553440677898</v>
+        <v>51.61698079429704</v>
       </c>
       <c r="P2" t="n">
-        <v>55.18918645844859</v>
+        <v>273</v>
       </c>
       <c r="Q2" t="n">
-        <v>76.65534407436202</v>
+        <v>60.21981092667988</v>
       </c>
       <c r="R2" t="n">
-        <v>107.6869287278782</v>
+        <v>420</v>
       </c>
       <c r="S2" t="n">
-        <v>76.65534407436202</v>
+        <v>68.82264105906272</v>
       </c>
       <c r="T2" t="n">
-        <v>210.1222243523014</v>
+        <v>665</v>
       </c>
       <c r="U2" t="n">
-        <v>76.65534407436202</v>
+        <v>77.42547119144557</v>
       </c>
       <c r="V2" t="n">
-        <v>409.9972920420831</v>
+        <v>1050</v>
       </c>
       <c r="W2" t="n">
-        <v>76.65534407436202</v>
+        <v>83.87759379073269</v>
       </c>
       <c r="X2" t="n">
-        <v>800.0000000000003</v>
+        <v>1400</v>
       </c>
       <c r="Y2" t="n">
-        <v>76.65534407436202</v>
+        <v>86.0283013238284</v>
       </c>
     </row>
     <row r="3">
@@ -648,70 +648,70 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="E3" t="n">
-        <v>48.57503142363934</v>
+        <v>10.18890893333379</v>
       </c>
       <c r="F3" t="n">
-        <v>1.951232399646889</v>
+        <v>17.5</v>
       </c>
       <c r="G3" t="n">
-        <v>91.83141735125876</v>
+        <v>40.75563573333517</v>
       </c>
       <c r="H3" t="n">
-        <v>3.807307877431757</v>
+        <v>38.5</v>
       </c>
       <c r="I3" t="n">
-        <v>160.7127312697541</v>
+        <v>61.13345360000274</v>
       </c>
       <c r="J3" t="n">
-        <v>7.428942485875671</v>
+        <v>73.50000000000001</v>
       </c>
       <c r="K3" t="n">
-        <v>231.7251355657886</v>
+        <v>81.51127146667034</v>
       </c>
       <c r="L3" t="n">
-        <v>14.49559327355391</v>
+        <v>119</v>
       </c>
       <c r="M3" t="n">
-        <v>259.9559531469213</v>
+        <v>101.8890893333379</v>
       </c>
       <c r="N3" t="n">
-        <v>28.28427124746191</v>
+        <v>182</v>
       </c>
       <c r="O3" t="n">
-        <v>262.225275130061</v>
+        <v>122.2669072000055</v>
       </c>
       <c r="P3" t="n">
-        <v>55.18918645844859</v>
+        <v>273</v>
       </c>
       <c r="Q3" t="n">
-        <v>262.2383330346097</v>
+        <v>142.6447250666731</v>
       </c>
       <c r="R3" t="n">
-        <v>107.6869287278782</v>
+        <v>420</v>
       </c>
       <c r="S3" t="n">
-        <v>262.2383335798603</v>
+        <v>163.0225429333407</v>
       </c>
       <c r="T3" t="n">
-        <v>210.1222243523014</v>
+        <v>665</v>
       </c>
       <c r="U3" t="n">
-        <v>262.2383335798603</v>
+        <v>183.4003608000082</v>
       </c>
       <c r="V3" t="n">
-        <v>409.9972920420831</v>
+        <v>1050</v>
       </c>
       <c r="W3" t="n">
-        <v>262.2383335798603</v>
+        <v>198.6837242000089</v>
       </c>
       <c r="X3" t="n">
-        <v>800.0000000000003</v>
+        <v>1400</v>
       </c>
       <c r="Y3" t="n">
-        <v>262.2383335798603</v>
+        <v>203.7781786666758</v>
       </c>
     </row>
     <row r="4">
@@ -728,67 +728,67 @@
         <v>1.661767947709472</v>
       </c>
       <c r="E4" t="n">
-        <v>10.37160160260147</v>
+        <v>10.11312199400586</v>
       </c>
       <c r="F4" t="n">
         <v>16.61767947709472</v>
       </c>
       <c r="G4" t="n">
-        <v>41.48640641040588</v>
+        <v>40.45248797602345</v>
       </c>
       <c r="H4" t="n">
         <v>35.85303843128415</v>
       </c>
       <c r="I4" t="n">
-        <v>62.22960961560882</v>
+        <v>60.67873196403517</v>
       </c>
       <c r="J4" t="n">
         <v>68.20607686256831</v>
       </c>
       <c r="K4" t="n">
-        <v>82.97281282081177</v>
+        <v>80.9049759520469</v>
       </c>
       <c r="L4" t="n">
         <v>110.1767947709472</v>
       </c>
       <c r="M4" t="n">
-        <v>103.7160160260147</v>
+        <v>101.1312199400586</v>
       </c>
       <c r="N4" t="n">
         <v>167.8828716335155</v>
       </c>
       <c r="O4" t="n">
-        <v>124.4592192312176</v>
+        <v>121.3574639280703</v>
       </c>
       <c r="P4" t="n">
         <v>252.7066279731785</v>
       </c>
       <c r="Q4" t="n">
-        <v>145.2024224364206</v>
+        <v>141.5837079160821</v>
       </c>
       <c r="R4" t="n">
         <v>388.2364611754099</v>
       </c>
       <c r="S4" t="n">
-        <v>165.9456256416235</v>
+        <v>161.8099519040938</v>
       </c>
       <c r="T4" t="n">
         <v>620.883973854736</v>
       </c>
       <c r="U4" t="n">
-        <v>186.6888288468265</v>
+        <v>182.0361958921055</v>
       </c>
       <c r="V4" t="n">
         <v>988.2375633966303</v>
       </c>
       <c r="W4" t="n">
-        <v>202.2462312507287</v>
+        <v>197.2058788831143</v>
       </c>
       <c r="X4" t="n">
         <v>1311.767947709472</v>
       </c>
       <c r="Y4" t="n">
-        <v>207.4320320520294</v>
+        <v>202.2624398801172</v>
       </c>
     </row>
     <row r="5">
@@ -805,67 +805,67 @@
         <v>1.465886659587723</v>
       </c>
       <c r="E5" t="n">
-        <v>11.99672237311677</v>
+        <v>11.7342762041225</v>
       </c>
       <c r="F5" t="n">
         <v>14.65886659587723</v>
       </c>
       <c r="G5" t="n">
-        <v>47.98688949246707</v>
+        <v>46.93710481649001</v>
       </c>
       <c r="H5" t="n">
         <v>29.97659978763169</v>
       </c>
       <c r="I5" t="n">
-        <v>71.98033423870059</v>
+        <v>70.40565722473501</v>
       </c>
       <c r="J5" t="n">
         <v>56.45319957526338</v>
       </c>
       <c r="K5" t="n">
-        <v>95.97377898493414</v>
+        <v>93.87420963298001</v>
       </c>
       <c r="L5" t="n">
         <v>90.58866595877231</v>
       </c>
       <c r="M5" t="n">
-        <v>119.9672237311677</v>
+        <v>117.342762041225</v>
       </c>
       <c r="N5" t="n">
         <v>136.5418655340357</v>
       </c>
       <c r="O5" t="n">
-        <v>143.9606684774012</v>
+        <v>140.81131444947</v>
       </c>
       <c r="P5" t="n">
         <v>207.6539317051763</v>
       </c>
       <c r="Q5" t="n">
-        <v>167.9541132236347</v>
+        <v>164.279866857715</v>
       </c>
       <c r="R5" t="n">
         <v>317.7191974515803</v>
       </c>
       <c r="S5" t="n">
-        <v>191.9475579698683</v>
+        <v>187.74841926596</v>
       </c>
       <c r="T5" t="n">
         <v>522.9433297938615</v>
       </c>
       <c r="U5" t="n">
-        <v>215.9410027161018</v>
+        <v>211.216971674205</v>
       </c>
       <c r="V5" t="n">
         <v>851.1206617114062</v>
       </c>
       <c r="W5" t="n">
-        <v>233.9360862757769</v>
+        <v>228.8183859803888</v>
       </c>
       <c r="X5" t="n">
         <v>1115.886659587723</v>
       </c>
       <c r="Y5" t="n">
-        <v>239.9344474623353</v>
+        <v>234.68552408245</v>
       </c>
     </row>
     <row r="6">
@@ -882,67 +882,67 @@
         <v>1.413756580239499</v>
       </c>
       <c r="E6" t="n">
-        <v>15.40568221032181</v>
+        <v>15.08195708119604</v>
       </c>
       <c r="F6" t="n">
         <v>14.137565802395</v>
       </c>
       <c r="G6" t="n">
-        <v>61.62272884128723</v>
+        <v>60.32782832478415</v>
       </c>
       <c r="H6" t="n">
         <v>28.41269740718498</v>
       </c>
       <c r="I6" t="n">
-        <v>92.43409326193084</v>
+        <v>90.49174248717623</v>
       </c>
       <c r="J6" t="n">
         <v>53.32539481436996</v>
       </c>
       <c r="K6" t="n">
-        <v>123.2454576825745</v>
+        <v>120.6556566495683</v>
       </c>
       <c r="L6" t="n">
         <v>85.37565802394995</v>
       </c>
       <c r="M6" t="n">
-        <v>154.0568221032181</v>
+        <v>150.8195708119604</v>
       </c>
       <c r="N6" t="n">
         <v>128.2010528383199</v>
       </c>
       <c r="O6" t="n">
-        <v>184.8681865238617</v>
+        <v>180.9834849743525</v>
       </c>
       <c r="P6" t="n">
         <v>195.6640134550849</v>
       </c>
       <c r="Q6" t="n">
-        <v>215.6795509445053</v>
+        <v>211.1473991367445</v>
       </c>
       <c r="R6" t="n">
         <v>298.9523688862198</v>
       </c>
       <c r="S6" t="n">
-        <v>246.4909153651489</v>
+        <v>241.3113132991366</v>
       </c>
       <c r="T6" t="n">
         <v>496.8782901197497</v>
       </c>
       <c r="U6" t="n">
-        <v>277.3022797857926</v>
+        <v>271.4752274615287</v>
       </c>
       <c r="V6" t="n">
         <v>814.6296061676496</v>
       </c>
       <c r="W6" t="n">
-        <v>300.4108031012752</v>
+        <v>294.0981630833227</v>
       </c>
       <c r="X6" t="n">
         <v>1063.756580239499</v>
       </c>
       <c r="Y6" t="n">
-        <v>308.1136442064362</v>
+        <v>301.6391416239208</v>
       </c>
     </row>
     <row r="7">
@@ -959,67 +959,67 @@
         <v>1.375195503436396</v>
       </c>
       <c r="E7" t="n">
-        <v>19.42797391645346</v>
+        <v>19.13971275652273</v>
       </c>
       <c r="F7" t="n">
         <v>13.75195503436396</v>
       </c>
       <c r="G7" t="n">
-        <v>77.71189566581383</v>
+        <v>76.55885102609093</v>
       </c>
       <c r="H7" t="n">
         <v>27.33027859278269</v>
       </c>
       <c r="I7" t="n">
-        <v>116.5678434987207</v>
+        <v>114.8382765391364</v>
       </c>
       <c r="J7" t="n">
         <v>51.01173020618376</v>
       </c>
       <c r="K7" t="n">
-        <v>155.4237913316277</v>
+        <v>153.1177020521819</v>
       </c>
       <c r="L7" t="n">
         <v>81.51955034363958</v>
       </c>
       <c r="M7" t="n">
-        <v>194.2797391645346</v>
+        <v>191.3971275652273</v>
       </c>
       <c r="N7" t="n">
         <v>122.5273704810954</v>
       </c>
       <c r="O7" t="n">
-        <v>233.1356869974415</v>
+        <v>229.6765530782728</v>
       </c>
       <c r="P7" t="n">
         <v>186.7949657903711</v>
       </c>
       <c r="Q7" t="n">
-        <v>271.9916348303483</v>
+        <v>267.9559785913182</v>
       </c>
       <c r="R7" t="n">
         <v>285.5664711683746</v>
       </c>
       <c r="S7" t="n">
-        <v>310.8475826632553</v>
+        <v>306.2354041043637</v>
       </c>
       <c r="T7" t="n">
         <v>475.6133919931096</v>
       </c>
       <c r="U7" t="n">
-        <v>349.7035304961622</v>
+        <v>344.5148296174092</v>
       </c>
       <c r="V7" t="n">
         <v>785.1564027491168</v>
       </c>
       <c r="W7" t="n">
-        <v>378.8454913708424</v>
+        <v>373.2243987521933</v>
       </c>
       <c r="X7" t="n">
         <v>1037.597751718198</v>
       </c>
       <c r="Y7" t="n">
-        <v>388.5594783290691</v>
+        <v>382.7942551304546</v>
       </c>
     </row>
     <row r="8">
@@ -1036,67 +1036,67 @@
         <v>1.238298502468788</v>
       </c>
       <c r="E8" t="n">
-        <v>21.68098044935765</v>
+        <v>21.37007004907905</v>
       </c>
       <c r="F8" t="n">
         <v>12.38298502468788</v>
       </c>
       <c r="G8" t="n">
-        <v>86.72392179743059</v>
+        <v>85.48028019631622</v>
       </c>
       <c r="H8" t="n">
         <v>23.63405956665726</v>
       </c>
       <c r="I8" t="n">
-        <v>130.0858826961459</v>
+        <v>128.2204202944743</v>
       </c>
       <c r="J8" t="n">
         <v>42.79791014812726</v>
       </c>
       <c r="K8" t="n">
-        <v>173.4478435948612</v>
+        <v>170.9605603926324</v>
       </c>
       <c r="L8" t="n">
         <v>67.82985024687876</v>
       </c>
       <c r="M8" t="n">
-        <v>216.8098044935765</v>
+        <v>213.7007004907905</v>
       </c>
       <c r="N8" t="n">
         <v>103.3617903456303</v>
       </c>
       <c r="O8" t="n">
-        <v>260.1717653922917</v>
+        <v>256.4408405889486</v>
       </c>
       <c r="P8" t="n">
         <v>155.3086555678212</v>
       </c>
       <c r="Q8" t="n">
-        <v>303.533726291007</v>
+        <v>299.1809806871067</v>
       </c>
       <c r="R8" t="n">
         <v>239.0214908393878</v>
       </c>
       <c r="S8" t="n">
-        <v>346.8956871897224</v>
+        <v>341.9211207852649</v>
       </c>
       <c r="T8" t="n">
         <v>396.2131314318969</v>
       </c>
       <c r="U8" t="n">
-        <v>390.2576480884376</v>
+        <v>384.6612608834229</v>
       </c>
       <c r="V8" t="n">
         <v>675.6388019750301</v>
       </c>
       <c r="W8" t="n">
-        <v>422.7791187624741</v>
+        <v>416.7163659570415</v>
       </c>
       <c r="X8" t="n">
         <v>969.1492512343938</v>
       </c>
       <c r="Y8" t="n">
-        <v>433.6196089871529</v>
+        <v>427.401400981581</v>
       </c>
     </row>
     <row r="9">
@@ -2034,70 +2034,70 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1.264786111430485</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>112.8355954523608</v>
+        <v>139.314019022959</v>
       </c>
       <c r="F21" t="n">
-        <v>12.64786111430485</v>
+        <v>1.951232399646889</v>
       </c>
       <c r="G21" t="n">
-        <v>451.3423818094431</v>
+        <v>271.5658930947487</v>
       </c>
       <c r="H21" t="n">
-        <v>24.3492250086231</v>
+        <v>3.807307877431757</v>
       </c>
       <c r="I21" t="n">
-        <v>677.0135727141645</v>
+        <v>527.9074967087423</v>
       </c>
       <c r="J21" t="n">
-        <v>44.38716668582911</v>
+        <v>7.428942485875671</v>
       </c>
       <c r="K21" t="n">
-        <v>902.6847636188861</v>
+        <v>1015.667836978981</v>
       </c>
       <c r="L21" t="n">
-        <v>70.47861114304851</v>
+        <v>14.49559327355391</v>
       </c>
       <c r="M21" t="n">
-        <v>1128.355954523608</v>
+        <v>1882.918496737477</v>
       </c>
       <c r="N21" t="n">
-        <v>107.0700556002679</v>
+        <v>28.28427124746191</v>
       </c>
       <c r="O21" t="n">
-        <v>1354.027145428329</v>
+        <v>3111.397860646721</v>
       </c>
       <c r="P21" t="n">
-        <v>161.4008056290116</v>
+        <v>55.18918645844859</v>
       </c>
       <c r="Q21" t="n">
-        <v>1579.698336333051</v>
+        <v>4057.747684397178</v>
       </c>
       <c r="R21" t="n">
-        <v>248.027277886365</v>
+        <v>107.6869287278782</v>
       </c>
       <c r="S21" t="n">
-        <v>1805.369527237772</v>
+        <v>4281.047496725331</v>
       </c>
       <c r="T21" t="n">
-        <v>411.5759446296815</v>
+        <v>210.1222243523014</v>
       </c>
       <c r="U21" t="n">
-        <v>2031.040718142494</v>
+        <v>4288.864893682803</v>
       </c>
       <c r="V21" t="n">
-        <v>696.8288891443881</v>
+        <v>409.9972920420831</v>
       </c>
       <c r="W21" t="n">
-        <v>2200.294111321035</v>
+        <v>4288.874960270813</v>
       </c>
       <c r="X21" t="n">
-        <v>982.3930557152424</v>
+        <v>800.0000000000003</v>
       </c>
       <c r="Y21" t="n">
-        <v>2256.711909047215</v>
+        <v>4288.874960293807</v>
       </c>
     </row>
     <row r="22">
@@ -2727,70 +2727,70 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>547.7929420766425</v>
+        <v>420.8343529178615</v>
       </c>
       <c r="F30" t="n">
-        <v>17.5</v>
+        <v>1.951232399646889</v>
       </c>
       <c r="G30" t="n">
-        <v>2191.17176830657</v>
+        <v>820.7575208015123</v>
       </c>
       <c r="H30" t="n">
-        <v>38.5</v>
+        <v>3.807307877431757</v>
       </c>
       <c r="I30" t="n">
-        <v>3286.757652459854</v>
+        <v>1598.613312383487</v>
       </c>
       <c r="J30" t="n">
-        <v>73.50000000000001</v>
+        <v>7.428942485875671</v>
       </c>
       <c r="K30" t="n">
-        <v>4382.34353661314</v>
+        <v>3098.124678878091</v>
       </c>
       <c r="L30" t="n">
-        <v>119</v>
+        <v>14.49559327355391</v>
       </c>
       <c r="M30" t="n">
-        <v>5477.929420766424</v>
+        <v>5894.058231620476</v>
       </c>
       <c r="N30" t="n">
-        <v>182</v>
+        <v>28.28427124746191</v>
       </c>
       <c r="O30" t="n">
-        <v>6573.515304919709</v>
+        <v>10523.32514446012</v>
       </c>
       <c r="P30" t="n">
-        <v>273</v>
+        <v>55.18918645844859</v>
       </c>
       <c r="Q30" t="n">
-        <v>7669.101189072993</v>
+        <v>15832.19130026525</v>
       </c>
       <c r="R30" t="n">
-        <v>420</v>
+        <v>107.6869287278782</v>
       </c>
       <c r="S30" t="n">
-        <v>8764.68707322628</v>
+        <v>18427.98799974247</v>
       </c>
       <c r="T30" t="n">
-        <v>665</v>
+        <v>210.1222243523014</v>
       </c>
       <c r="U30" t="n">
-        <v>9860.272957379564</v>
+        <v>18718.11816084078</v>
       </c>
       <c r="V30" t="n">
-        <v>1050</v>
+        <v>409.9972920420831</v>
       </c>
       <c r="W30" t="n">
-        <v>10681.96237049453</v>
+        <v>18721.0687485998</v>
       </c>
       <c r="X30" t="n">
-        <v>1400</v>
+        <v>800.0000000000003</v>
       </c>
       <c r="Y30" t="n">
-        <v>10955.85884153285</v>
+        <v>18721.06911736049</v>
       </c>
     </row>
     <row r="31">
@@ -3112,70 +3112,70 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>639.0344851085556</v>
+        <v>462.7721669531539</v>
       </c>
       <c r="F35" t="n">
-        <v>17.5</v>
+        <v>1.951232399646889</v>
       </c>
       <c r="G35" t="n">
-        <v>2556.137940434222</v>
+        <v>902.6790581605367</v>
       </c>
       <c r="H35" t="n">
-        <v>38.5</v>
+        <v>3.807307877431757</v>
       </c>
       <c r="I35" t="n">
-        <v>3834.206910651333</v>
+        <v>1759.134500363581</v>
       </c>
       <c r="J35" t="n">
-        <v>73.50000000000001</v>
+        <v>7.428942485875671</v>
       </c>
       <c r="K35" t="n">
-        <v>5112.275880868445</v>
+        <v>3416.238094534586</v>
       </c>
       <c r="L35" t="n">
-        <v>119</v>
+        <v>14.49559327355391</v>
       </c>
       <c r="M35" t="n">
-        <v>6390.344851085555</v>
+        <v>6548.43617580144</v>
       </c>
       <c r="N35" t="n">
-        <v>182</v>
+        <v>28.28427124746191</v>
       </c>
       <c r="O35" t="n">
-        <v>7668.413821302665</v>
+        <v>11987.10563008828</v>
       </c>
       <c r="P35" t="n">
-        <v>273</v>
+        <v>55.18918645844859</v>
       </c>
       <c r="Q35" t="n">
-        <v>8946.482791519777</v>
+        <v>19149.1471830594</v>
       </c>
       <c r="R35" t="n">
-        <v>420</v>
+        <v>107.6869287278782</v>
       </c>
       <c r="S35" t="n">
-        <v>10224.55176173689</v>
+        <v>23825.74128113274</v>
       </c>
       <c r="T35" t="n">
-        <v>665</v>
+        <v>210.1222243523014</v>
       </c>
       <c r="U35" t="n">
-        <v>11502.620731954</v>
+        <v>24661.63266252984</v>
       </c>
       <c r="V35" t="n">
-        <v>1050</v>
+        <v>409.9972920420831</v>
       </c>
       <c r="W35" t="n">
-        <v>12461.17245961683</v>
+        <v>24680.27022052712</v>
       </c>
       <c r="X35" t="n">
-        <v>1400</v>
+        <v>800.0000000000003</v>
       </c>
       <c r="Y35" t="n">
-        <v>12780.68970217111</v>
+        <v>24680.28057479898</v>
       </c>
     </row>
     <row r="36">
@@ -3189,70 +3189,70 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="E36" t="n">
-        <v>634.9391578102676</v>
+        <v>941.2269562516105</v>
       </c>
       <c r="F36" t="n">
-        <v>1.951232399646889</v>
+        <v>17.5</v>
       </c>
       <c r="G36" t="n">
-        <v>1238.407995744216</v>
+        <v>3764.907825006442</v>
       </c>
       <c r="H36" t="n">
-        <v>3.807307877431757</v>
+        <v>38.5</v>
       </c>
       <c r="I36" t="n">
-        <v>2412.672629850178</v>
+        <v>5647.361737509663</v>
       </c>
       <c r="J36" t="n">
-        <v>7.428942485875671</v>
+        <v>73.50000000000001</v>
       </c>
       <c r="K36" t="n">
-        <v>4680.080123829017</v>
+        <v>7529.815650012884</v>
       </c>
       <c r="L36" t="n">
-        <v>14.49559327355391</v>
+        <v>119</v>
       </c>
       <c r="M36" t="n">
-        <v>8933.603897919031</v>
+        <v>9412.269562516105</v>
       </c>
       <c r="N36" t="n">
-        <v>28.28427124746191</v>
+        <v>182</v>
       </c>
       <c r="O36" t="n">
-        <v>16126.05537522721</v>
+        <v>11294.72347501933</v>
       </c>
       <c r="P36" t="n">
-        <v>55.18918645844859</v>
+        <v>273</v>
       </c>
       <c r="Q36" t="n">
-        <v>24884.15416878762</v>
+        <v>13177.17738752255</v>
       </c>
       <c r="R36" t="n">
-        <v>107.6869287278782</v>
+        <v>420</v>
       </c>
       <c r="S36" t="n">
-        <v>29722.73113733198</v>
+        <v>15059.63130002577</v>
       </c>
       <c r="T36" t="n">
-        <v>210.1222243523014</v>
+        <v>665</v>
       </c>
       <c r="U36" t="n">
-        <v>30380.90514197214</v>
+        <v>16942.08521252899</v>
       </c>
       <c r="V36" t="n">
-        <v>409.9972920420831</v>
+        <v>1050</v>
       </c>
       <c r="W36" t="n">
-        <v>30390.23524249446</v>
+        <v>18353.92564690641</v>
       </c>
       <c r="X36" t="n">
-        <v>800.0000000000003</v>
+        <v>1400</v>
       </c>
       <c r="Y36" t="n">
-        <v>30390.23744203538</v>
+        <v>18824.53912503221</v>
       </c>
     </row>
     <row r="37">
@@ -3266,70 +3266,70 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
-        <v>690.3803833129862</v>
+        <v>487.8574002671367</v>
       </c>
       <c r="F37" t="n">
-        <v>17.5</v>
+        <v>1.951232399646889</v>
       </c>
       <c r="G37" t="n">
-        <v>2761.521533251945</v>
+        <v>951.6408736174644</v>
       </c>
       <c r="H37" t="n">
-        <v>38.5</v>
+        <v>3.807307877431757</v>
       </c>
       <c r="I37" t="n">
-        <v>4142.282299877917</v>
+        <v>1854.778955711186</v>
       </c>
       <c r="J37" t="n">
-        <v>73.50000000000001</v>
+        <v>7.428942485875671</v>
       </c>
       <c r="K37" t="n">
-        <v>5523.043066503889</v>
+        <v>3603.652567361725</v>
       </c>
       <c r="L37" t="n">
-        <v>119</v>
+        <v>14.49559327355391</v>
       </c>
       <c r="M37" t="n">
-        <v>6903.803833129861</v>
+        <v>6919.542965443232</v>
       </c>
       <c r="N37" t="n">
-        <v>182</v>
+        <v>28.28427124746191</v>
       </c>
       <c r="O37" t="n">
-        <v>8284.564599755833</v>
+        <v>12740.70442792607</v>
       </c>
       <c r="P37" t="n">
-        <v>273</v>
+        <v>55.18918645844859</v>
       </c>
       <c r="Q37" t="n">
-        <v>9665.325366381805</v>
+        <v>20666.84162284768</v>
       </c>
       <c r="R37" t="n">
-        <v>420</v>
+        <v>107.6869287278782</v>
       </c>
       <c r="S37" t="n">
-        <v>11046.08613300778</v>
+        <v>26242.17759915199</v>
       </c>
       <c r="T37" t="n">
-        <v>665</v>
+        <v>210.1222243523014</v>
       </c>
       <c r="U37" t="n">
-        <v>12426.84689963375</v>
+        <v>27370.11646823052</v>
       </c>
       <c r="V37" t="n">
-        <v>1050</v>
+        <v>409.9972920420831</v>
       </c>
       <c r="W37" t="n">
-        <v>13462.41747460323</v>
+        <v>27400.9040131797</v>
       </c>
       <c r="X37" t="n">
-        <v>1400</v>
+        <v>800.0000000000003</v>
       </c>
       <c r="Y37" t="n">
-        <v>13807.60766625972</v>
+        <v>27400.92899553424</v>
       </c>
     </row>
     <row r="38">
@@ -3651,70 +3651,70 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="E42" t="n">
-        <v>651.4001929407057</v>
+        <v>984.7802905163544</v>
       </c>
       <c r="F42" t="n">
-        <v>1.951232399646889</v>
+        <v>17.5</v>
       </c>
       <c r="G42" t="n">
-        <v>1270.688513033202</v>
+        <v>3939.121162065418</v>
       </c>
       <c r="H42" t="n">
-        <v>3.807307877431757</v>
+        <v>38.5</v>
       </c>
       <c r="I42" t="n">
-        <v>2476.852222142752</v>
+        <v>5908.681743098126</v>
       </c>
       <c r="J42" t="n">
-        <v>7.428942485875671</v>
+        <v>73.50000000000001</v>
       </c>
       <c r="K42" t="n">
-        <v>4814.035570709894</v>
+        <v>7878.242324130835</v>
       </c>
       <c r="L42" t="n">
-        <v>14.49559327355391</v>
+        <v>119</v>
       </c>
       <c r="M42" t="n">
-        <v>9256.157844653118</v>
+        <v>9847.802905163544</v>
       </c>
       <c r="N42" t="n">
-        <v>28.28427124746191</v>
+        <v>182</v>
       </c>
       <c r="O42" t="n">
-        <v>17122.49341316478</v>
+        <v>11817.36348619625</v>
       </c>
       <c r="P42" t="n">
-        <v>55.18918645844859</v>
+        <v>273</v>
       </c>
       <c r="Q42" t="n">
-        <v>28125.21477664772</v>
+        <v>13786.92406722896</v>
       </c>
       <c r="R42" t="n">
-        <v>107.6869287278782</v>
+        <v>420</v>
       </c>
       <c r="S42" t="n">
-        <v>36355.14749465895</v>
+        <v>15756.48464826167</v>
       </c>
       <c r="T42" t="n">
-        <v>210.1222243523014</v>
+        <v>665</v>
       </c>
       <c r="U42" t="n">
-        <v>38202.01519392437</v>
+        <v>17726.04522929438</v>
       </c>
       <c r="V42" t="n">
-        <v>409.9972920420831</v>
+        <v>1050</v>
       </c>
       <c r="W42" t="n">
-        <v>38261.64588227093</v>
+        <v>19203.21566506891</v>
       </c>
       <c r="X42" t="n">
-        <v>800.0000000000003</v>
+        <v>1400</v>
       </c>
       <c r="Y42" t="n">
-        <v>38261.71200185318</v>
+        <v>19695.60581032709</v>
       </c>
     </row>
     <row r="43">
@@ -3805,70 +3805,70 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="E44" t="n">
-        <v>814.4686438328331</v>
+        <v>1328.923985919506</v>
       </c>
       <c r="F44" t="n">
-        <v>1.951232399646889</v>
+        <v>17.5</v>
       </c>
       <c r="G44" t="n">
-        <v>1588.79649644758</v>
+        <v>5315.695943678023</v>
       </c>
       <c r="H44" t="n">
-        <v>3.807307877431757</v>
+        <v>38.5</v>
       </c>
       <c r="I44" t="n">
-        <v>3096.987575393132</v>
+        <v>7973.543915517033</v>
       </c>
       <c r="J44" t="n">
-        <v>7.428942485875671</v>
+        <v>73.50000000000001</v>
       </c>
       <c r="K44" t="n">
-        <v>6019.871527785859</v>
+        <v>10631.39188735605</v>
       </c>
       <c r="L44" t="n">
-        <v>14.49559327355391</v>
+        <v>119</v>
       </c>
       <c r="M44" t="n">
-        <v>11578.48515738811</v>
+        <v>13289.23985919506</v>
       </c>
       <c r="N44" t="n">
-        <v>28.28427124746191</v>
+        <v>182</v>
       </c>
       <c r="O44" t="n">
-        <v>21442.87715131309</v>
+        <v>15947.08783103407</v>
       </c>
       <c r="P44" t="n">
-        <v>55.18918645844859</v>
+        <v>273</v>
       </c>
       <c r="Q44" t="n">
-        <v>35332.09830165873</v>
+        <v>18604.93580287308</v>
       </c>
       <c r="R44" t="n">
-        <v>107.6869287278782</v>
+        <v>420</v>
       </c>
       <c r="S44" t="n">
-        <v>45882.19872799428</v>
+        <v>21262.78377471209</v>
       </c>
       <c r="T44" t="n">
-        <v>210.1222243523014</v>
+        <v>665</v>
       </c>
       <c r="U44" t="n">
-        <v>48312.54201186045</v>
+        <v>23920.6317465511</v>
       </c>
       <c r="V44" t="n">
-        <v>409.9972920420831</v>
+        <v>1050</v>
       </c>
       <c r="W44" t="n">
-        <v>48394.39741628983</v>
+        <v>25914.01772543036</v>
       </c>
       <c r="X44" t="n">
-        <v>800.0000000000003</v>
+        <v>1400</v>
       </c>
       <c r="Y44" t="n">
-        <v>48394.49555779635</v>
+        <v>26578.47971839011</v>
       </c>
     </row>
     <row r="45">
@@ -3882,70 +3882,70 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>1194.054870645135</v>
+        <v>753.0170541702568</v>
       </c>
       <c r="F45" t="n">
-        <v>17.5</v>
+        <v>1.951232399646889</v>
       </c>
       <c r="G45" t="n">
-        <v>4776.219482580541</v>
+        <v>1468.970227876105</v>
       </c>
       <c r="H45" t="n">
-        <v>38.5</v>
+        <v>3.807307877431757</v>
       </c>
       <c r="I45" t="n">
-        <v>7164.329223870812</v>
+        <v>2863.772082700163</v>
       </c>
       <c r="J45" t="n">
-        <v>73.50000000000001</v>
+        <v>7.428942485875671</v>
       </c>
       <c r="K45" t="n">
-        <v>9552.438965161082</v>
+        <v>5569.183347451703</v>
       </c>
       <c r="L45" t="n">
-        <v>119</v>
+        <v>14.49559327355391</v>
       </c>
       <c r="M45" t="n">
-        <v>11940.54870645135</v>
+        <v>10730.48015477292</v>
       </c>
       <c r="N45" t="n">
-        <v>182</v>
+        <v>28.28427124746191</v>
       </c>
       <c r="O45" t="n">
-        <v>14328.65844774162</v>
+        <v>19994.42715727854</v>
       </c>
       <c r="P45" t="n">
-        <v>273</v>
+        <v>55.18918645844859</v>
       </c>
       <c r="Q45" t="n">
-        <v>16716.76818903189</v>
+        <v>33515.1753750662</v>
       </c>
       <c r="R45" t="n">
-        <v>420</v>
+        <v>107.6869287278782</v>
       </c>
       <c r="S45" t="n">
-        <v>19104.87793032216</v>
+        <v>44697.02683904086</v>
       </c>
       <c r="T45" t="n">
-        <v>665</v>
+        <v>210.1222243523014</v>
       </c>
       <c r="U45" t="n">
-        <v>21492.98767161243</v>
+        <v>47679.51214757744</v>
       </c>
       <c r="V45" t="n">
-        <v>1050</v>
+        <v>409.9972920420831</v>
       </c>
       <c r="W45" t="n">
-        <v>23284.06997758014</v>
+        <v>47806.61222245733</v>
       </c>
       <c r="X45" t="n">
-        <v>1400</v>
+        <v>800.0000000000003</v>
       </c>
       <c r="Y45" t="n">
-        <v>23881.09741290271</v>
+        <v>47806.84704283991</v>
       </c>
     </row>
     <row r="46">
@@ -4036,70 +4036,70 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="E47" t="n">
-        <v>915.0342820437734</v>
+        <v>1569.949304764902</v>
       </c>
       <c r="F47" t="n">
-        <v>1.951232399646889</v>
+        <v>17.5</v>
       </c>
       <c r="G47" t="n">
-        <v>1785.032701371566</v>
+        <v>6279.797219059608</v>
       </c>
       <c r="H47" t="n">
-        <v>3.807307877431757</v>
+        <v>38.5</v>
       </c>
       <c r="I47" t="n">
-        <v>3479.958198182846</v>
+        <v>9419.695828589412</v>
       </c>
       <c r="J47" t="n">
-        <v>7.428942485875671</v>
+        <v>73.50000000000001</v>
       </c>
       <c r="K47" t="n">
-        <v>6767.622882094262</v>
+        <v>12559.59443811922</v>
       </c>
       <c r="L47" t="n">
-        <v>14.49559327355391</v>
+        <v>119</v>
       </c>
       <c r="M47" t="n">
-        <v>13040.59822231356</v>
+        <v>15699.49304764902</v>
       </c>
       <c r="N47" t="n">
-        <v>28.28427124746191</v>
+        <v>182</v>
       </c>
       <c r="O47" t="n">
-        <v>24305.55308844956</v>
+        <v>18839.39165717882</v>
       </c>
       <c r="P47" t="n">
-        <v>55.18918645844859</v>
+        <v>273</v>
       </c>
       <c r="Q47" t="n">
-        <v>40773.24664941157</v>
+        <v>21979.29026670863</v>
       </c>
       <c r="R47" t="n">
-        <v>107.6869287278782</v>
+        <v>420</v>
       </c>
       <c r="S47" t="n">
-        <v>54445.21607258629</v>
+        <v>25119.18887623843</v>
       </c>
       <c r="T47" t="n">
-        <v>210.1222243523014</v>
+        <v>665</v>
       </c>
       <c r="U47" t="n">
-        <v>58116.64871342134</v>
+        <v>28259.08748576824</v>
       </c>
       <c r="V47" t="n">
-        <v>409.9972920420831</v>
+        <v>1050</v>
       </c>
       <c r="W47" t="n">
-        <v>58274.81143331033</v>
+        <v>30614.01144291559</v>
       </c>
       <c r="X47" t="n">
-        <v>800.0000000000003</v>
+        <v>1400</v>
       </c>
       <c r="Y47" t="n">
-        <v>58275.1094749173</v>
+        <v>31398.98609529804</v>
       </c>
     </row>
     <row r="48">
@@ -4498,70 +4498,70 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>1.286145577660908</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>483.6993642737864</v>
+        <v>367.196085783462</v>
       </c>
       <c r="F53" t="n">
-        <v>12.86145577660908</v>
+        <v>1.951232399646889</v>
       </c>
       <c r="G53" t="n">
-        <v>1934.797457095146</v>
+        <v>716.3960026991288</v>
       </c>
       <c r="H53" t="n">
-        <v>24.92593059684451</v>
+        <v>3.807307877431757</v>
       </c>
       <c r="I53" t="n">
-        <v>2902.196185642718</v>
+        <v>1397.195153869669</v>
       </c>
       <c r="J53" t="n">
-        <v>45.66873465965447</v>
+        <v>7.428942485875671</v>
       </c>
       <c r="K53" t="n">
-        <v>3869.594914190291</v>
+        <v>2721.363137896133</v>
       </c>
       <c r="L53" t="n">
-        <v>72.61455776609077</v>
+        <v>14.49559327355391</v>
       </c>
       <c r="M53" t="n">
-        <v>4836.993642737863</v>
+        <v>5274.062199832274</v>
       </c>
       <c r="N53" t="n">
-        <v>110.0603808725271</v>
+        <v>28.28427124746191</v>
       </c>
       <c r="O53" t="n">
-        <v>5804.392371285436</v>
+        <v>10033.96835887713</v>
       </c>
       <c r="P53" t="n">
-        <v>166.3134828620088</v>
+        <v>55.18918645844859</v>
       </c>
       <c r="Q53" t="n">
-        <v>6771.791099833008</v>
+        <v>17916.36606744033</v>
       </c>
       <c r="R53" t="n">
-        <v>255.2894964047086</v>
+        <v>107.6869287278782</v>
       </c>
       <c r="S53" t="n">
-        <v>7739.189828380582</v>
+        <v>26960.29476161373</v>
       </c>
       <c r="T53" t="n">
-        <v>423.9644350433265</v>
+        <v>210.1222243523014</v>
       </c>
       <c r="U53" t="n">
-        <v>8706.588556928155</v>
+        <v>31386.63162686837</v>
       </c>
       <c r="V53" t="n">
-        <v>713.9164621287262</v>
+        <v>409.9972920420831</v>
       </c>
       <c r="W53" t="n">
-        <v>9432.137603338833</v>
+        <v>31882.12339392172</v>
       </c>
       <c r="X53" t="n">
-        <v>993.0727888304538</v>
+        <v>800.0000000000003</v>
       </c>
       <c r="Y53" t="n">
-        <v>9673.987285475727</v>
+        <v>31887.1757483055</v>
       </c>
     </row>
     <row r="54">
@@ -5730,70 +5730,70 @@
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>1.465274406054907</v>
+        <v>1</v>
       </c>
       <c r="E69" t="n">
-        <v>921.7476906697361</v>
+        <v>552.9415535739973</v>
       </c>
       <c r="F69" t="n">
-        <v>14.65274406054908</v>
+        <v>1.951232399646889</v>
       </c>
       <c r="G69" t="n">
-        <v>3686.990762678945</v>
+        <v>1078.827829382286</v>
       </c>
       <c r="H69" t="n">
-        <v>29.95823218164723</v>
+        <v>3.807307877431757</v>
       </c>
       <c r="I69" t="n">
-        <v>5530.486144018416</v>
+        <v>2104.378165405696</v>
       </c>
       <c r="J69" t="n">
-        <v>56.41646436329445</v>
+        <v>7.428942485875671</v>
       </c>
       <c r="K69" t="n">
-        <v>7373.981525357889</v>
+        <v>4101.194797458433</v>
       </c>
       <c r="L69" t="n">
-        <v>90.52744060549075</v>
+        <v>14.49559327355391</v>
       </c>
       <c r="M69" t="n">
-        <v>9217.47690669736</v>
+        <v>7965.967358358159</v>
       </c>
       <c r="N69" t="n">
-        <v>136.4439049687852</v>
+        <v>28.28427124746191</v>
       </c>
       <c r="O69" t="n">
-        <v>11060.97228803683</v>
+        <v>15279.87196370718</v>
       </c>
       <c r="P69" t="n">
-        <v>207.5131133926287</v>
+        <v>55.18918645844859</v>
       </c>
       <c r="Q69" t="n">
-        <v>12904.4676693763</v>
+        <v>28034.15281737316</v>
       </c>
       <c r="R69" t="n">
-        <v>317.4987861797667</v>
+        <v>107.6869287278782</v>
       </c>
       <c r="S69" t="n">
-        <v>14747.96305071578</v>
+        <v>45049.48106306994</v>
       </c>
       <c r="T69" t="n">
-        <v>522.6372030274538</v>
+        <v>210.1222243523014</v>
       </c>
       <c r="U69" t="n">
-        <v>16591.45843205525</v>
+        <v>56483.30226542398</v>
       </c>
       <c r="V69" t="n">
-        <v>850.6920842384352</v>
+        <v>409.9972920420831</v>
       </c>
       <c r="W69" t="n">
-        <v>17974.07996805985</v>
+        <v>58626.50656896612</v>
       </c>
       <c r="X69" t="n">
-        <v>1115.274406054908</v>
+        <v>800.0000000000003</v>
       </c>
       <c r="Y69" t="n">
-        <v>18434.95381339472</v>
+        <v>58678.1629277765</v>
       </c>
     </row>
     <row r="70">

</xml_diff>